<commit_message>
upload results & validation analysis
</commit_message>
<xml_diff>
--- a/Tables/rd_sett.xlsx
+++ b/Tables/rd_sett.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\rd_information_bargaining\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851A0259-322E-4BFF-BFC1-2B216472B6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928F3FD1-CEAF-4584-B9CF-BE579535A9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8190" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9C778B-4ACA-4509-AF6F-10D310567EB0}"/>
+    <workbookView xWindow="4905" yWindow="450" windowWidth="21600" windowHeight="11175" xr2:uid="{2B9C778B-4ACA-4509-AF6F-10D310567EB0}"/>
   </bookViews>
   <sheets>
     <sheet name="rd_sett_" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
   <si>
     <t>Effective observations [L , R]</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>III s I</t>
+  </si>
+  <si>
+    <t>III vs I</t>
   </si>
 </sst>
 </file>
@@ -296,43 +299,43 @@
             <v>0.408*</v>
           </cell>
           <cell r="C5" t="str">
-            <v>0.499**</v>
+            <v>0.426**</v>
           </cell>
           <cell r="D5" t="str">
             <v>0.338</v>
           </cell>
           <cell r="E5" t="str">
-            <v>0.293</v>
+            <v>0.302</v>
           </cell>
           <cell r="F5" t="str">
             <v>0.397**</v>
           </cell>
           <cell r="G5" t="str">
-            <v>0.359**</v>
+            <v>0.388***</v>
           </cell>
           <cell r="H5" t="str">
             <v>-0.248</v>
           </cell>
           <cell r="I5" t="str">
-            <v>-0.353</v>
+            <v>-0.344</v>
           </cell>
           <cell r="J5" t="str">
             <v>-0.0273</v>
           </cell>
           <cell r="K5" t="str">
-            <v>-0.0777</v>
+            <v>0.243</v>
           </cell>
           <cell r="L5" t="str">
             <v>-0.179</v>
           </cell>
           <cell r="M5" t="str">
-            <v>-0.237</v>
+            <v>-0.222</v>
           </cell>
           <cell r="N5" t="str">
             <v>0.338</v>
           </cell>
           <cell r="O5" t="str">
-            <v>0.490**</v>
+            <v>0.512**</v>
           </cell>
         </row>
         <row r="6">
@@ -349,37 +352,37 @@
             <v>(0.209)</v>
           </cell>
           <cell r="E6" t="str">
-            <v>(0.217)</v>
+            <v>(0.224)</v>
           </cell>
           <cell r="F6" t="str">
             <v>(0.158)</v>
           </cell>
           <cell r="G6" t="str">
-            <v>(0.150)</v>
+            <v>(0.149)</v>
           </cell>
           <cell r="H6" t="str">
             <v>(0.166)</v>
           </cell>
           <cell r="I6" t="str">
-            <v>(1,517)</v>
+            <v>(1,622)</v>
           </cell>
           <cell r="J6" t="str">
             <v>(0.161)</v>
           </cell>
           <cell r="K6" t="str">
-            <v>(2,673)</v>
+            <v>(0.212)</v>
           </cell>
           <cell r="L6" t="str">
             <v>(0.127)</v>
           </cell>
           <cell r="M6" t="str">
-            <v>(0.147)</v>
+            <v>(0.140)</v>
           </cell>
           <cell r="N6" t="str">
             <v>(0.225)</v>
           </cell>
           <cell r="O6" t="str">
-            <v>(0.220)</v>
+            <v>(0.224)</v>
           </cell>
         </row>
         <row r="9">
@@ -390,43 +393,43 @@
             <v>0.447*</v>
           </cell>
           <cell r="C9" t="str">
-            <v>0.558**</v>
+            <v>0.469**</v>
           </cell>
           <cell r="D9" t="str">
             <v>0.324</v>
           </cell>
           <cell r="E9" t="str">
-            <v>0.205</v>
+            <v>0.227</v>
           </cell>
           <cell r="F9" t="str">
             <v>0.420**</v>
           </cell>
           <cell r="G9" t="str">
-            <v>0.353**</v>
+            <v>0.387**</v>
           </cell>
           <cell r="H9" t="str">
             <v>-0.325</v>
           </cell>
           <cell r="I9" t="str">
-            <v>-0.350</v>
+            <v>-0.342</v>
           </cell>
           <cell r="J9" t="str">
             <v>0.0190</v>
           </cell>
           <cell r="K9" t="str">
-            <v>-0.0259</v>
+            <v>0.396</v>
           </cell>
           <cell r="L9" t="str">
             <v>-0.231</v>
           </cell>
           <cell r="M9" t="str">
-            <v>-0.229</v>
+            <v>-0.215</v>
           </cell>
           <cell r="N9" t="str">
             <v>0.385</v>
           </cell>
           <cell r="O9" t="str">
-            <v>0.541**</v>
+            <v>0.567**</v>
           </cell>
         </row>
         <row r="10">
@@ -443,25 +446,25 @@
             <v>(0.242)</v>
           </cell>
           <cell r="E10" t="str">
-            <v>(0.256)</v>
+            <v>(0.263)</v>
           </cell>
           <cell r="F10" t="str">
             <v>(0.183)</v>
           </cell>
           <cell r="G10" t="str">
-            <v>(0.174)</v>
+            <v>(0.173)</v>
           </cell>
           <cell r="H10" t="str">
             <v>(0.205)</v>
           </cell>
           <cell r="I10" t="str">
-            <v>(2,074)</v>
+            <v>(2,194)</v>
           </cell>
           <cell r="J10" t="str">
             <v>(0.196)</v>
           </cell>
           <cell r="K10" t="str">
-            <v>(3,389)</v>
+            <v>(0.274)</v>
           </cell>
           <cell r="L10" t="str">
             <v>(0.152)</v>
@@ -473,7 +476,7 @@
             <v>(0.275)</v>
           </cell>
           <cell r="O10" t="str">
-            <v>(0.259)</v>
+            <v>(0.265)</v>
           </cell>
         </row>
         <row r="16">
@@ -481,43 +484,43 @@
             <v>1.112</v>
           </cell>
           <cell r="C16" t="str">
-            <v>1.226</v>
+            <v>1.212</v>
           </cell>
           <cell r="D16" t="str">
             <v>1.166</v>
           </cell>
           <cell r="E16" t="str">
-            <v>0.910</v>
+            <v>1.050</v>
           </cell>
           <cell r="F16" t="str">
             <v>1.067</v>
           </cell>
           <cell r="G16" t="str">
-            <v>1.115</v>
+            <v>1.105</v>
           </cell>
           <cell r="H16" t="str">
             <v>41.71</v>
           </cell>
           <cell r="I16" t="str">
-            <v>30.86</v>
+            <v>31.60</v>
           </cell>
           <cell r="J16" t="str">
             <v>67</v>
           </cell>
           <cell r="K16" t="str">
-            <v>82.93</v>
+            <v>37.37</v>
           </cell>
           <cell r="L16" t="str">
             <v>42.28</v>
           </cell>
           <cell r="M16" t="str">
-            <v>30.49</v>
+            <v>33.46</v>
           </cell>
           <cell r="N16" t="str">
             <v>0.634</v>
           </cell>
           <cell r="O16" t="str">
-            <v>0.583</v>
+            <v>0.569</v>
           </cell>
           <cell r="P16" t="str">
             <v>0.182</v>
@@ -531,43 +534,43 @@
             <v>1.112</v>
           </cell>
           <cell r="C17" t="str">
-            <v>1.226</v>
+            <v>1.212</v>
           </cell>
           <cell r="D17" t="str">
             <v>1.166</v>
           </cell>
           <cell r="E17" t="str">
-            <v>0.910</v>
+            <v>1.050</v>
           </cell>
           <cell r="F17" t="str">
             <v>1.067</v>
           </cell>
           <cell r="G17" t="str">
-            <v>1.115</v>
+            <v>1.105</v>
           </cell>
           <cell r="H17" t="str">
             <v>41.71</v>
           </cell>
           <cell r="I17" t="str">
-            <v>30.86</v>
+            <v>31.60</v>
           </cell>
           <cell r="J17" t="str">
             <v>67</v>
           </cell>
           <cell r="K17" t="str">
-            <v>82.93</v>
+            <v>37.37</v>
           </cell>
           <cell r="L17" t="str">
             <v>42.28</v>
           </cell>
           <cell r="M17" t="str">
-            <v>30.49</v>
+            <v>33.46</v>
           </cell>
           <cell r="N17" t="str">
             <v>0.634</v>
           </cell>
           <cell r="O17" t="str">
-            <v>0.583</v>
+            <v>0.569</v>
           </cell>
           <cell r="P17" t="str">
             <v>0.182</v>
@@ -581,43 +584,43 @@
             <v>65</v>
           </cell>
           <cell r="C18" t="str">
-            <v>67</v>
+            <v>66</v>
           </cell>
           <cell r="D18" t="str">
             <v>51</v>
           </cell>
           <cell r="E18" t="str">
-            <v>38</v>
+            <v>45</v>
           </cell>
           <cell r="F18" t="str">
             <v>109</v>
           </cell>
           <cell r="G18" t="str">
-            <v>108</v>
+            <v>107</v>
           </cell>
           <cell r="H18" t="str">
             <v>98</v>
           </cell>
           <cell r="I18" t="str">
-            <v>65</v>
+            <v>68</v>
           </cell>
           <cell r="J18" t="str">
             <v>62</v>
           </cell>
           <cell r="K18" t="str">
-            <v>73</v>
+            <v>31</v>
           </cell>
           <cell r="L18" t="str">
             <v>137</v>
           </cell>
           <cell r="M18" t="str">
-            <v>89</v>
+            <v>103</v>
           </cell>
           <cell r="N18" t="str">
             <v>146</v>
           </cell>
           <cell r="O18" t="str">
-            <v>123</v>
+            <v>120</v>
           </cell>
           <cell r="P18" t="str">
             <v>14</v>
@@ -631,13 +634,13 @@
             <v>42</v>
           </cell>
           <cell r="C19" t="str">
-            <v>43</v>
+            <v>42</v>
           </cell>
           <cell r="D19" t="str">
             <v>21</v>
           </cell>
           <cell r="E19" t="str">
-            <v>15</v>
+            <v>17</v>
           </cell>
           <cell r="F19" t="str">
             <v>61</v>
@@ -655,19 +658,19 @@
             <v>58</v>
           </cell>
           <cell r="K19" t="str">
-            <v>68</v>
+            <v>35</v>
           </cell>
           <cell r="L19" t="str">
             <v>111</v>
           </cell>
           <cell r="M19" t="str">
-            <v>89</v>
+            <v>93</v>
           </cell>
           <cell r="N19" t="str">
             <v>44</v>
           </cell>
           <cell r="O19" t="str">
-            <v>35</v>
+            <v>34</v>
           </cell>
           <cell r="P19" t="str">
             <v>7</v>
@@ -721,43 +724,43 @@
             <v>-0.435*</v>
           </cell>
           <cell r="C5" t="str">
-            <v>-0.521**</v>
+            <v>-0.337</v>
           </cell>
           <cell r="D5" t="str">
             <v>-0.145</v>
           </cell>
           <cell r="E5" t="str">
-            <v>-0.589***</v>
+            <v>-0.306</v>
           </cell>
           <cell r="F5" t="str">
             <v>-0.367**</v>
           </cell>
           <cell r="G5" t="str">
-            <v>-0.363**</v>
+            <v>-0.370**</v>
           </cell>
           <cell r="H5" t="str">
             <v>0.216</v>
           </cell>
           <cell r="I5" t="str">
-            <v>0.124</v>
+            <v>0.227</v>
           </cell>
           <cell r="J5" t="str">
             <v>-0.175</v>
           </cell>
           <cell r="K5" t="str">
-            <v>-0.108</v>
+            <v>-0.290</v>
           </cell>
           <cell r="L5" t="str">
             <v>0.0645</v>
           </cell>
           <cell r="M5" t="str">
-            <v>0.0417</v>
+            <v>0.0609</v>
           </cell>
           <cell r="N5" t="str">
             <v>0.223</v>
           </cell>
           <cell r="O5" t="str">
-            <v>-0.416</v>
+            <v>0.180</v>
           </cell>
         </row>
         <row r="6">
@@ -768,13 +771,13 @@
             <v>(0.227)</v>
           </cell>
           <cell r="C6" t="str">
-            <v>(0.242)</v>
+            <v>(0.219)</v>
           </cell>
           <cell r="D6" t="str">
             <v>(0.315)</v>
           </cell>
           <cell r="E6" t="str">
-            <v>(0.131)</v>
+            <v>(0.215)</v>
           </cell>
           <cell r="F6" t="str">
             <v>(0.179)</v>
@@ -786,25 +789,25 @@
             <v>(0.172)</v>
           </cell>
           <cell r="I6" t="str">
-            <v>(1,654)</v>
+            <v>(14.88)</v>
           </cell>
           <cell r="J6" t="str">
             <v>(0.219)</v>
           </cell>
           <cell r="K6" t="str">
-            <v>(0.186)</v>
+            <v>(0.218)</v>
           </cell>
           <cell r="L6" t="str">
             <v>(0.121)</v>
           </cell>
           <cell r="M6" t="str">
-            <v>(592.2)</v>
+            <v>(0.0993)</v>
           </cell>
           <cell r="N6" t="str">
             <v>(0.289)</v>
           </cell>
           <cell r="O6" t="str">
-            <v>(0.319)</v>
+            <v>(0.313)</v>
           </cell>
         </row>
         <row r="9">
@@ -815,43 +818,43 @@
             <v>-0.510**</v>
           </cell>
           <cell r="C9" t="str">
-            <v>-0.638**</v>
+            <v>-0.429*</v>
           </cell>
           <cell r="D9" t="str">
             <v>-0.172</v>
           </cell>
           <cell r="E9" t="str">
-            <v>-0.838***</v>
+            <v>-0.450</v>
           </cell>
           <cell r="F9" t="str">
             <v>-0.430**</v>
           </cell>
           <cell r="G9" t="str">
-            <v>-0.433**</v>
+            <v>-0.443**</v>
           </cell>
           <cell r="H9" t="str">
             <v>0.246</v>
           </cell>
           <cell r="I9" t="str">
-            <v>0.0496</v>
+            <v>0.252</v>
           </cell>
           <cell r="J9" t="str">
             <v>-0.223</v>
           </cell>
           <cell r="K9" t="str">
-            <v>-0.128</v>
+            <v>-0.392</v>
           </cell>
           <cell r="L9" t="str">
             <v>0.0731</v>
           </cell>
           <cell r="M9" t="str">
-            <v>0.0176</v>
+            <v>0.0759</v>
           </cell>
           <cell r="N9" t="str">
             <v>0.216</v>
           </cell>
           <cell r="O9" t="str">
-            <v>-0.591</v>
+            <v>0.129</v>
           </cell>
         </row>
         <row r="10">
@@ -862,13 +865,13 @@
             <v>(0.252)</v>
           </cell>
           <cell r="C10" t="str">
-            <v>(0.276)</v>
+            <v>(0.251)</v>
           </cell>
           <cell r="D10" t="str">
             <v>(0.379)</v>
           </cell>
           <cell r="E10" t="str">
-            <v>(0.226)</v>
+            <v>(0.286)</v>
           </cell>
           <cell r="F10" t="str">
             <v>(0.199)</v>
@@ -880,25 +883,25 @@
             <v>(0.215)</v>
           </cell>
           <cell r="I10" t="str">
-            <v>(2,053)</v>
+            <v>(18.39)</v>
           </cell>
           <cell r="J10" t="str">
             <v>(0.273)</v>
           </cell>
           <cell r="K10" t="str">
-            <v>(0.213)</v>
+            <v>(0.278)</v>
           </cell>
           <cell r="L10" t="str">
             <v>(0.148)</v>
           </cell>
           <cell r="M10" t="str">
-            <v>(747.1)</v>
+            <v>(0.114)</v>
           </cell>
           <cell r="N10" t="str">
             <v>(0.357)</v>
           </cell>
           <cell r="O10" t="str">
-            <v>(0.378)</v>
+            <v>(0.385)</v>
           </cell>
         </row>
         <row r="16">
@@ -906,49 +909,49 @@
             <v>0.736</v>
           </cell>
           <cell r="C16" t="str">
-            <v>0.721</v>
+            <v>0.784</v>
           </cell>
           <cell r="D16" t="str">
             <v>1.128</v>
           </cell>
           <cell r="E16" t="str">
-            <v>0.790</v>
+            <v>1.001</v>
           </cell>
           <cell r="F16" t="str">
             <v>1.008</v>
           </cell>
           <cell r="G16" t="str">
-            <v>0.872</v>
+            <v>0.831</v>
           </cell>
           <cell r="H16" t="str">
             <v>59.33</v>
           </cell>
           <cell r="I16" t="str">
-            <v>37.85</v>
+            <v>55.18</v>
           </cell>
           <cell r="J16" t="str">
             <v>63.01</v>
           </cell>
           <cell r="K16" t="str">
-            <v>95.60</v>
+            <v>43.70</v>
           </cell>
           <cell r="L16" t="str">
             <v>65.75</v>
           </cell>
           <cell r="M16" t="str">
-            <v>55.74</v>
+            <v>109.3</v>
           </cell>
           <cell r="N16" t="str">
             <v>0.821</v>
           </cell>
           <cell r="O16" t="str">
-            <v>0.376</v>
+            <v>0.673</v>
           </cell>
           <cell r="P16" t="str">
             <v>0.186</v>
           </cell>
           <cell r="Q16" t="str">
-            <v>0.212</v>
+            <v>0.218</v>
           </cell>
         </row>
         <row r="17">
@@ -956,49 +959,49 @@
             <v>0.736</v>
           </cell>
           <cell r="C17" t="str">
-            <v>0.721</v>
+            <v>0.784</v>
           </cell>
           <cell r="D17" t="str">
             <v>1.128</v>
           </cell>
           <cell r="E17" t="str">
-            <v>0.790</v>
+            <v>1.001</v>
           </cell>
           <cell r="F17" t="str">
             <v>1.008</v>
           </cell>
           <cell r="G17" t="str">
-            <v>0.872</v>
+            <v>0.831</v>
           </cell>
           <cell r="H17" t="str">
             <v>59.33</v>
           </cell>
           <cell r="I17" t="str">
-            <v>37.85</v>
+            <v>55.18</v>
           </cell>
           <cell r="J17" t="str">
             <v>63.01</v>
           </cell>
           <cell r="K17" t="str">
-            <v>95.60</v>
+            <v>43.70</v>
           </cell>
           <cell r="L17" t="str">
             <v>65.75</v>
           </cell>
           <cell r="M17" t="str">
-            <v>55.74</v>
+            <v>109.3</v>
           </cell>
           <cell r="N17" t="str">
             <v>0.821</v>
           </cell>
           <cell r="O17" t="str">
-            <v>0.376</v>
+            <v>0.673</v>
           </cell>
           <cell r="P17" t="str">
             <v>0.186</v>
           </cell>
           <cell r="Q17" t="str">
-            <v>0.212</v>
+            <v>0.218</v>
           </cell>
         </row>
         <row r="18">
@@ -1006,49 +1009,49 @@
             <v>19</v>
           </cell>
           <cell r="C18" t="str">
-            <v>19</v>
+            <v>22</v>
           </cell>
           <cell r="D18" t="str">
             <v>29</v>
           </cell>
           <cell r="E18" t="str">
-            <v>20</v>
+            <v>24</v>
           </cell>
           <cell r="F18" t="str">
             <v>58</v>
           </cell>
           <cell r="G18" t="str">
-            <v>46</v>
+            <v>45</v>
           </cell>
           <cell r="H18" t="str">
             <v>99</v>
           </cell>
           <cell r="I18" t="str">
-            <v>62</v>
+            <v>95</v>
           </cell>
           <cell r="J18" t="str">
             <v>47</v>
           </cell>
           <cell r="K18" t="str">
-            <v>51</v>
+            <v>30</v>
           </cell>
           <cell r="L18" t="str">
             <v>160</v>
           </cell>
           <cell r="M18" t="str">
-            <v>134</v>
+            <v>191</v>
           </cell>
           <cell r="N18" t="str">
             <v>97</v>
           </cell>
           <cell r="O18" t="str">
-            <v>22</v>
+            <v>83</v>
           </cell>
           <cell r="P18" t="str">
             <v>7</v>
           </cell>
           <cell r="Q18" t="str">
-            <v>11</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="19">
@@ -1056,43 +1059,43 @@
             <v>24</v>
           </cell>
           <cell r="C19" t="str">
-            <v>22</v>
+            <v>23</v>
           </cell>
           <cell r="D19" t="str">
             <v>19</v>
           </cell>
           <cell r="E19" t="str">
-            <v>9</v>
+            <v>11</v>
           </cell>
           <cell r="F19" t="str">
             <v>44</v>
           </cell>
           <cell r="G19" t="str">
-            <v>36</v>
+            <v>35</v>
           </cell>
           <cell r="H19" t="str">
             <v>49</v>
           </cell>
           <cell r="I19" t="str">
-            <v>28</v>
+            <v>40</v>
           </cell>
           <cell r="J19" t="str">
             <v>45</v>
           </cell>
           <cell r="K19" t="str">
-            <v>55</v>
+            <v>32</v>
           </cell>
           <cell r="L19" t="str">
             <v>95</v>
           </cell>
           <cell r="M19" t="str">
-            <v>89</v>
+            <v>132</v>
           </cell>
           <cell r="N19" t="str">
             <v>38</v>
           </cell>
           <cell r="O19" t="str">
-            <v>15</v>
+            <v>32</v>
           </cell>
           <cell r="P19" t="str">
             <v>8</v>
@@ -1406,24 +1409,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789015B5-DACC-4F22-891E-C89EA2122BE5}">
   <dimension ref="A2:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:F60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.90625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.26953125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="19" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.28515625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="8" t="s">
         <v>4</v>
@@ -1436,7 +1439,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>5</v>
@@ -1449,7 +1452,7 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
@@ -1463,7 +1466,7 @@
       </c>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="str">
         <f>[1]Sheet1!A2</f>
         <v/>
@@ -1495,7 +1498,7 @@
         <v>(6)</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>[1]Sheet1!A5</f>
         <v>Conventional</v>
@@ -1506,7 +1509,7 @@
       </c>
       <c r="C6" s="1" t="str">
         <f>[1]Sheet1!C5</f>
-        <v>0.499**</v>
+        <v>0.426**</v>
       </c>
       <c r="E6" s="1" t="str">
         <f>[1]Sheet1!D5</f>
@@ -1514,7 +1517,7 @@
       </c>
       <c r="F6" s="1" t="str">
         <f>[1]Sheet1!E5</f>
-        <v>0.293</v>
+        <v>0.302</v>
       </c>
       <c r="H6" s="1" t="str">
         <f>[1]Sheet1!F5</f>
@@ -1522,10 +1525,10 @@
       </c>
       <c r="I6" s="1" t="str">
         <f>[1]Sheet1!G5</f>
-        <v>0.359**</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.388***</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>[1]Sheet1!A6</f>
         <v/>
@@ -1544,7 +1547,7 @@
       </c>
       <c r="F7" s="1" t="str">
         <f>[1]Sheet1!E6</f>
-        <v>(0.217)</v>
+        <v>(0.224)</v>
       </c>
       <c r="H7" s="1" t="str">
         <f>[1]Sheet1!F6</f>
@@ -1552,10 +1555,10 @@
       </c>
       <c r="I7" s="1" t="str">
         <f>[1]Sheet1!G6</f>
-        <v>(0.150)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>(0.149)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>[1]Sheet1!A9</f>
         <v>Robust</v>
@@ -1566,7 +1569,7 @@
       </c>
       <c r="C8" s="1" t="str">
         <f>[1]Sheet1!C9</f>
-        <v>0.558**</v>
+        <v>0.469**</v>
       </c>
       <c r="E8" s="1" t="str">
         <f>[1]Sheet1!D9</f>
@@ -1574,7 +1577,7 @@
       </c>
       <c r="F8" s="1" t="str">
         <f>[1]Sheet1!E9</f>
-        <v>0.205</v>
+        <v>0.227</v>
       </c>
       <c r="H8" s="1" t="str">
         <f>[1]Sheet1!F9</f>
@@ -1582,10 +1585,10 @@
       </c>
       <c r="I8" s="1" t="str">
         <f>[1]Sheet1!G9</f>
-        <v>0.353**</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.387**</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>[1]Sheet1!A10</f>
         <v/>
@@ -1604,7 +1607,7 @@
       </c>
       <c r="F9" s="1" t="str">
         <f>[1]Sheet1!E10</f>
-        <v>(0.256)</v>
+        <v>(0.263)</v>
       </c>
       <c r="H9" s="1" t="str">
         <f>[1]Sheet1!F10</f>
@@ -1612,10 +1615,10 @@
       </c>
       <c r="I9" s="1" t="str">
         <f>[1]Sheet1!G10</f>
-        <v>(0.174)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>(0.173)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>0</v>
       </c>
@@ -1625,7 +1628,7 @@
       </c>
       <c r="C11" s="7" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!C18," ,  ",[1]Sheet1!C19,"]")</f>
-        <v>[67 ,  43]</v>
+        <v>[66 ,  42]</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="str">
@@ -1634,7 +1637,7 @@
       </c>
       <c r="F11" s="7" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!E18," ,  ",[1]Sheet1!E19,"]")</f>
-        <v>[38 ,  15]</v>
+        <v>[45 ,  17]</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7" t="str">
@@ -1643,10 +1646,10 @@
       </c>
       <c r="I11" s="7" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!G18," ,  ",[1]Sheet1!G19,"]")</f>
-        <v>[108 ,  57]</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>[107 ,  57]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1656,7 +1659,7 @@
       </c>
       <c r="C12" s="6" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!C16," ,  ",[1]Sheet1!C17,"]")</f>
-        <v>[1.226 ,  1.226]</v>
+        <v>[1.212 ,  1.212]</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="str">
@@ -1665,7 +1668,7 @@
       </c>
       <c r="F12" s="6" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!E16," ,  ",[1]Sheet1!E17,"]")</f>
-        <v>[0.910 ,  0.910]</v>
+        <v>[1.050 ,  1.050]</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6" t="str">
@@ -1674,11 +1677,11 @@
       </c>
       <c r="I12" s="6" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!G16," ,  ",[1]Sheet1!G17,"]")</f>
-        <v>[1.115 ,  1.115]</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>[1.105 ,  1.105]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="8" t="s">
         <v>6</v>
@@ -1691,7 +1694,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>3</v>
       </c>
@@ -1705,7 +1708,7 @@
       </c>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="str">
         <f>[2]Sheet1!A2</f>
         <v/>
@@ -1731,7 +1734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>[2]Sheet1!A5</f>
         <v>Conventional</v>
@@ -1742,7 +1745,7 @@
       </c>
       <c r="C17" s="1" t="str">
         <f>[2]Sheet1!C5</f>
-        <v>-0.521**</v>
+        <v>-0.337</v>
       </c>
       <c r="E17" s="1" t="str">
         <f>[2]Sheet1!D5</f>
@@ -1750,7 +1753,7 @@
       </c>
       <c r="F17" s="1" t="str">
         <f>[2]Sheet1!E5</f>
-        <v>-0.589***</v>
+        <v>-0.306</v>
       </c>
       <c r="H17" s="1" t="str">
         <f>[2]Sheet1!F5</f>
@@ -1758,10 +1761,10 @@
       </c>
       <c r="I17" s="1" t="str">
         <f>[2]Sheet1!G5</f>
-        <v>-0.363**</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>-0.370**</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>[2]Sheet1!A6</f>
         <v/>
@@ -1772,7 +1775,7 @@
       </c>
       <c r="C18" s="1" t="str">
         <f>[2]Sheet1!C6</f>
-        <v>(0.242)</v>
+        <v>(0.219)</v>
       </c>
       <c r="E18" s="1" t="str">
         <f>[2]Sheet1!D6</f>
@@ -1780,7 +1783,7 @@
       </c>
       <c r="F18" s="1" t="str">
         <f>[2]Sheet1!E6</f>
-        <v>(0.131)</v>
+        <v>(0.215)</v>
       </c>
       <c r="H18" s="1" t="str">
         <f>[2]Sheet1!F6</f>
@@ -1791,7 +1794,7 @@
         <v>(0.176)</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>[2]Sheet1!A9</f>
         <v>Robust</v>
@@ -1802,7 +1805,7 @@
       </c>
       <c r="C19" s="1" t="str">
         <f>[2]Sheet1!C9</f>
-        <v>-0.638**</v>
+        <v>-0.429*</v>
       </c>
       <c r="E19" s="1" t="str">
         <f>[2]Sheet1!D9</f>
@@ -1810,7 +1813,7 @@
       </c>
       <c r="F19" s="1" t="str">
         <f>[2]Sheet1!E9</f>
-        <v>-0.838***</v>
+        <v>-0.450</v>
       </c>
       <c r="H19" s="1" t="str">
         <f>[2]Sheet1!F9</f>
@@ -1818,10 +1821,10 @@
       </c>
       <c r="I19" s="1" t="str">
         <f>[2]Sheet1!G9</f>
-        <v>-0.433**</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>-0.443**</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>[2]Sheet1!A10</f>
         <v/>
@@ -1832,7 +1835,7 @@
       </c>
       <c r="C20" s="1" t="str">
         <f>[2]Sheet1!C10</f>
-        <v>(0.276)</v>
+        <v>(0.251)</v>
       </c>
       <c r="E20" s="1" t="str">
         <f>[2]Sheet1!D10</f>
@@ -1840,7 +1843,7 @@
       </c>
       <c r="F20" s="1" t="str">
         <f>[2]Sheet1!E10</f>
-        <v>(0.226)</v>
+        <v>(0.286)</v>
       </c>
       <c r="H20" s="1" t="str">
         <f>[2]Sheet1!F10</f>
@@ -1851,7 +1854,7 @@
         <v>(0.204)</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>0</v>
       </c>
@@ -1861,7 +1864,7 @@
       </c>
       <c r="C22" s="7" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!C18," ,  ",[2]Sheet1!C19,"]")</f>
-        <v>[19 ,  22]</v>
+        <v>[22 ,  23]</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="str">
@@ -1870,7 +1873,7 @@
       </c>
       <c r="F22" s="7" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!E18," ,  ",[2]Sheet1!E19,"]")</f>
-        <v>[20 ,  9]</v>
+        <v>[24 ,  11]</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7" t="str">
@@ -1879,10 +1882,10 @@
       </c>
       <c r="I22" s="7" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!G18," ,  ",[2]Sheet1!G19,"]")</f>
-        <v>[46 ,  36]</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>[45 ,  35]</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
@@ -1892,7 +1895,7 @@
       </c>
       <c r="C23" s="6" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!C16," ,  ",[2]Sheet1!C17,"]")</f>
-        <v>[0.721 ,  0.721]</v>
+        <v>[0.784 ,  0.784]</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="str">
@@ -1901,7 +1904,7 @@
       </c>
       <c r="F23" s="6" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!E16," ,  ",[2]Sheet1!E17,"]")</f>
-        <v>[0.790 ,  0.790]</v>
+        <v>[1.001 ,  1.001]</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6" t="str">
@@ -1910,11 +1913,11 @@
       </c>
       <c r="I23" s="6" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!G16," ,  ",[2]Sheet1!G17,"]")</f>
-        <v>[0.872 ,  0.872]</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>[0.831 ,  0.831]</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="8" t="s">
         <v>7</v>
@@ -1927,7 +1930,7 @@
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="10" t="s">
         <v>5</v>
@@ -1940,7 +1943,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
         <v>8</v>
       </c>
@@ -1954,7 +1957,7 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="6" t="s">
         <v>18</v>
@@ -1977,7 +1980,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1987,7 +1990,7 @@
       </c>
       <c r="C30" s="1" t="str">
         <f>[1]Sheet1!I5</f>
-        <v>-0.353</v>
+        <v>-0.344</v>
       </c>
       <c r="E30" s="1" t="str">
         <f>[1]Sheet1!J5</f>
@@ -1995,7 +1998,7 @@
       </c>
       <c r="F30" s="1" t="str">
         <f>[1]Sheet1!K5</f>
-        <v>-0.0777</v>
+        <v>0.243</v>
       </c>
       <c r="H30" s="1" t="str">
         <f>[1]Sheet1!L5</f>
@@ -2003,10 +2006,10 @@
       </c>
       <c r="I30" s="1" t="str">
         <f>[1]Sheet1!M5</f>
-        <v>-0.237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>-0.222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -2016,7 +2019,7 @@
       </c>
       <c r="C31" s="1" t="str">
         <f>[1]Sheet1!I6</f>
-        <v>(1,517)</v>
+        <v>(1,622)</v>
       </c>
       <c r="E31" s="1" t="str">
         <f>[1]Sheet1!J6</f>
@@ -2024,7 +2027,7 @@
       </c>
       <c r="F31" s="1" t="str">
         <f>[1]Sheet1!K6</f>
-        <v>(2,673)</v>
+        <v>(0.212)</v>
       </c>
       <c r="H31" s="1" t="str">
         <f>[1]Sheet1!L6</f>
@@ -2032,10 +2035,10 @@
       </c>
       <c r="I31" s="1" t="str">
         <f>[1]Sheet1!M6</f>
-        <v>(0.147)</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+        <v>(0.140)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -2045,7 +2048,7 @@
       </c>
       <c r="C32" s="1" t="str">
         <f>[1]Sheet1!I9</f>
-        <v>-0.350</v>
+        <v>-0.342</v>
       </c>
       <c r="E32" s="1" t="str">
         <f>[1]Sheet1!J9</f>
@@ -2053,7 +2056,7 @@
       </c>
       <c r="F32" s="1" t="str">
         <f>[1]Sheet1!K9</f>
-        <v>-0.0259</v>
+        <v>0.396</v>
       </c>
       <c r="H32" s="1" t="str">
         <f>[1]Sheet1!L9</f>
@@ -2061,10 +2064,10 @@
       </c>
       <c r="I32" s="1" t="str">
         <f>[1]Sheet1!M9</f>
-        <v>-0.229</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+        <v>-0.215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -2074,7 +2077,7 @@
       </c>
       <c r="C33" s="1" t="str">
         <f>[1]Sheet1!I10</f>
-        <v>(2,074)</v>
+        <v>(2,194)</v>
       </c>
       <c r="E33" s="1" t="str">
         <f>[1]Sheet1!J10</f>
@@ -2082,7 +2085,7 @@
       </c>
       <c r="F33" s="1" t="str">
         <f>[1]Sheet1!K10</f>
-        <v>(3,389)</v>
+        <v>(0.274)</v>
       </c>
       <c r="H33" s="1" t="str">
         <f>[1]Sheet1!L10</f>
@@ -2093,7 +2096,7 @@
         <v>(0.182)</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>0</v>
       </c>
@@ -2103,7 +2106,7 @@
       </c>
       <c r="C35" s="7" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!I18," ,  ",[1]Sheet1!I19,"]")</f>
-        <v>[65 ,  59]</v>
+        <v>[68 ,  59]</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7" t="str">
@@ -2112,7 +2115,7 @@
       </c>
       <c r="F35" s="7" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!K18," ,  ",[1]Sheet1!K19,"]")</f>
-        <v>[73 ,  68]</v>
+        <v>[31 ,  35]</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7" t="str">
@@ -2121,10 +2124,10 @@
       </c>
       <c r="I35" s="7" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!M18," ,  ",[1]Sheet1!M19,"]")</f>
-        <v>[89 ,  89]</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>[103 ,  93]</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>1</v>
       </c>
@@ -2134,7 +2137,7 @@
       </c>
       <c r="C36" s="6" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!I16," ,  ",[1]Sheet1!I17,"]")</f>
-        <v>[30.86 ,  30.86]</v>
+        <v>[31.60 ,  31.60]</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6" t="str">
@@ -2143,7 +2146,7 @@
       </c>
       <c r="F36" s="6" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!K16," ,  ",[1]Sheet1!K17,"]")</f>
-        <v>[82.93 ,  82.93]</v>
+        <v>[37.37 ,  37.37]</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6" t="str">
@@ -2152,11 +2155,11 @@
       </c>
       <c r="I36" s="6" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!M16," ,  ",[1]Sheet1!M17,"]")</f>
-        <v>[30.49 ,  30.49]</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>[33.46 ,  33.46]</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="8" t="s">
         <v>6</v>
@@ -2169,7 +2172,7 @@
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>8</v>
       </c>
@@ -2183,7 +2186,7 @@
       </c>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>25</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>(12)</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -2224,7 +2227,7 @@
       </c>
       <c r="C41" s="1" t="str">
         <f>[2]Sheet1!I5</f>
-        <v>0.124</v>
+        <v>0.227</v>
       </c>
       <c r="E41" s="1" t="str">
         <f>[2]Sheet1!J5</f>
@@ -2232,7 +2235,7 @@
       </c>
       <c r="F41" s="1" t="str">
         <f>[2]Sheet1!K5</f>
-        <v>-0.108</v>
+        <v>-0.290</v>
       </c>
       <c r="H41" s="1" t="str">
         <f>[2]Sheet1!L5</f>
@@ -2240,10 +2243,10 @@
       </c>
       <c r="I41" s="1" t="str">
         <f>[2]Sheet1!M5</f>
-        <v>0.0417</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.0609</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -2253,7 +2256,7 @@
       </c>
       <c r="C42" s="1" t="str">
         <f>[2]Sheet1!I6</f>
-        <v>(1,654)</v>
+        <v>(14.88)</v>
       </c>
       <c r="E42" s="1" t="str">
         <f>[2]Sheet1!J6</f>
@@ -2261,7 +2264,7 @@
       </c>
       <c r="F42" s="1" t="str">
         <f>[2]Sheet1!K6</f>
-        <v>(0.186)</v>
+        <v>(0.218)</v>
       </c>
       <c r="H42" s="1" t="str">
         <f>[2]Sheet1!L6</f>
@@ -2269,10 +2272,10 @@
       </c>
       <c r="I42" s="1" t="str">
         <f>[2]Sheet1!M6</f>
-        <v>(592.2)</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+        <v>(0.0993)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -2282,7 +2285,7 @@
       </c>
       <c r="C43" s="1" t="str">
         <f>[2]Sheet1!I9</f>
-        <v>0.0496</v>
+        <v>0.252</v>
       </c>
       <c r="E43" s="1" t="str">
         <f>[2]Sheet1!J9</f>
@@ -2290,7 +2293,7 @@
       </c>
       <c r="F43" s="1" t="str">
         <f>[2]Sheet1!K9</f>
-        <v>-0.128</v>
+        <v>-0.392</v>
       </c>
       <c r="H43" s="1" t="str">
         <f>[2]Sheet1!L9</f>
@@ -2298,10 +2301,10 @@
       </c>
       <c r="I43" s="1" t="str">
         <f>[2]Sheet1!M9</f>
-        <v>0.0176</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.0759</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -2311,7 +2314,7 @@
       </c>
       <c r="C44" s="1" t="str">
         <f>[2]Sheet1!I10</f>
-        <v>(2,053)</v>
+        <v>(18.39)</v>
       </c>
       <c r="E44" s="1" t="str">
         <f>[2]Sheet1!J10</f>
@@ -2319,7 +2322,7 @@
       </c>
       <c r="F44" s="1" t="str">
         <f>[2]Sheet1!K10</f>
-        <v>(0.213)</v>
+        <v>(0.278)</v>
       </c>
       <c r="H44" s="1" t="str">
         <f>[2]Sheet1!L10</f>
@@ -2327,10 +2330,10 @@
       </c>
       <c r="I44" s="1" t="str">
         <f>[2]Sheet1!M10</f>
-        <v>(747.1)</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+        <v>(0.114)</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>0</v>
       </c>
@@ -2340,7 +2343,7 @@
       </c>
       <c r="C46" s="7" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!I18," ,  ",[2]Sheet1!I19,"]")</f>
-        <v>[62 ,  28]</v>
+        <v>[95 ,  40]</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7" t="str">
@@ -2349,7 +2352,7 @@
       </c>
       <c r="F46" s="7" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!K18," ,  ",[2]Sheet1!K19,"]")</f>
-        <v>[51 ,  55]</v>
+        <v>[30 ,  32]</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7" t="str">
@@ -2358,10 +2361,10 @@
       </c>
       <c r="I46" s="7" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!M18," ,  ",[2]Sheet1!M19,"]")</f>
-        <v>[134 ,  89]</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>[191 ,  132]</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>1</v>
       </c>
@@ -2371,7 +2374,7 @@
       </c>
       <c r="C47" s="6" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!I16," ,  ",[2]Sheet1!I17,"]")</f>
-        <v>[37.85 ,  37.85]</v>
+        <v>[55.18 ,  55.18]</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6" t="str">
@@ -2380,7 +2383,7 @@
       </c>
       <c r="F47" s="6" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!K16," ,  ",[2]Sheet1!K17,"]")</f>
-        <v>[95.60 ,  95.60]</v>
+        <v>[43.70 ,  43.70]</v>
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="6" t="str">
@@ -2389,11 +2392,11 @@
       </c>
       <c r="I47" s="6" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!M16," ,  ",[2]Sheet1!M17,"]")</f>
-        <v>[55.74 ,  55.74]</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>[109.3 ,  109.3]</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="8" t="s">
         <v>28</v>
@@ -2403,7 +2406,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="10" t="s">
         <v>5</v>
@@ -2413,17 +2416,17 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C52" s="9"/>
       <c r="E52" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F52" s="9"/>
     </row>
-    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="6" t="s">
         <v>18</v>
@@ -2439,7 +2442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -2449,7 +2452,7 @@
       </c>
       <c r="C54" s="1" t="str">
         <f>[1]Sheet1!O5</f>
-        <v>0.490**</v>
+        <v>0.512**</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>27</v>
@@ -2458,7 +2461,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -2468,10 +2471,10 @@
       </c>
       <c r="C55" s="1" t="str">
         <f>[1]Sheet1!O6</f>
-        <v>(0.220)</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+        <v>(0.224)</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -2481,7 +2484,7 @@
       </c>
       <c r="C56" s="1" t="str">
         <f>[1]Sheet1!O9</f>
-        <v>0.541**</v>
+        <v>0.567**</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>27</v>
@@ -2490,17 +2493,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="str">
         <f>[1]Sheet1!N10</f>
         <v>(0.275)</v>
       </c>
       <c r="C57" s="1" t="str">
         <f>[1]Sheet1!O10</f>
-        <v>(0.259)</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+        <v>(0.265)</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>0</v>
       </c>
@@ -2510,7 +2513,7 @@
       </c>
       <c r="C59" s="7" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!O18," ,  ",[1]Sheet1!O19,"]")</f>
-        <v>[123 ,  35]</v>
+        <v>[120 ,  34]</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="7" t="str">
@@ -2522,7 +2525,7 @@
         <v>[14 ,  7]</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>1</v>
       </c>
@@ -2532,7 +2535,7 @@
       </c>
       <c r="C60" s="6" t="str">
         <f>_xlfn.CONCAT("[",[1]Sheet1!O16," ,  ",[1]Sheet1!O17,"]")</f>
-        <v>[0.583 ,  0.583]</v>
+        <v>[0.569 ,  0.569]</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="6" t="str">
@@ -2544,8 +2547,8 @@
         <v>[0.190 ,  0.190]</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="62" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="8" t="s">
         <v>6</v>
@@ -2555,7 +2558,7 @@
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="9" t="s">
         <v>29</v>
       </c>
@@ -2565,7 +2568,7 @@
       </c>
       <c r="F63" s="9"/>
     </row>
-    <row r="64" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="6" t="s">
         <v>22</v>
@@ -2581,7 +2584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -2591,7 +2594,7 @@
       </c>
       <c r="C65" s="1" t="str">
         <f>[2]Sheet1!O5</f>
-        <v>-0.416</v>
+        <v>0.180</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>27</v>
@@ -2600,7 +2603,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2610,10 +2613,10 @@
       </c>
       <c r="C66" s="1" t="str">
         <f>[2]Sheet1!O6</f>
-        <v>(0.319)</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+        <v>(0.313)</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -2623,7 +2626,7 @@
       </c>
       <c r="C67" s="1" t="str">
         <f>[2]Sheet1!O9</f>
-        <v>-0.591</v>
+        <v>0.129</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>27</v>
@@ -2632,7 +2635,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>25</v>
       </c>
@@ -2642,10 +2645,10 @@
       </c>
       <c r="C68" s="1" t="str">
         <f>[2]Sheet1!O10</f>
-        <v>(0.378)</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+        <v>(0.385)</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>0</v>
       </c>
@@ -2655,7 +2658,7 @@
       </c>
       <c r="C70" s="7" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!O18," ,  ",[2]Sheet1!O19,"]")</f>
-        <v>[22 ,  15]</v>
+        <v>[83 ,  32]</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="7" t="str">
@@ -2664,10 +2667,10 @@
       </c>
       <c r="F70" s="7" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!Q18," ,  ",[2]Sheet1!Q19,"]")</f>
-        <v>[11 ,  9]</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>[12 ,  9]</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>1</v>
       </c>
@@ -2677,7 +2680,7 @@
       </c>
       <c r="C71" s="6" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!O16," ,  ",[2]Sheet1!O17,"]")</f>
-        <v>[0.376 ,  0.376]</v>
+        <v>[0.673 ,  0.673]</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="6" t="str">
@@ -2686,10 +2689,10 @@
       </c>
       <c r="F71" s="6" t="str">
         <f>_xlfn.CONCAT("[",[2]Sheet1!Q16," ,  ",[2]Sheet1!Q17,"]")</f>
-        <v>[0.212 ,  0.212]</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>[0.218 ,  0.218]</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
     <mergeCell ref="B14:I14"/>

</xml_diff>